<commit_message>
criando função de executar o script e adicionar os dados dentro da planilha automaticamente
</commit_message>
<xml_diff>
--- a/Prestador/neomater/resultado/relatorio_neomater_APENAS_VALORES.xlsx
+++ b/Prestador/neomater/resultado/relatorio_neomater_APENAS_VALORES.xlsx
@@ -461,40 +461,40 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L2" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -727,13 +727,13 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B9" t="n">
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
         <v>1</v>
@@ -742,30 +742,30 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B10" t="n">
         <v>0</v>
@@ -774,36 +774,36 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B11" t="n">
         <v>0</v>
@@ -812,25 +812,25 @@
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
         <v>0</v>
@@ -906,13 +906,13 @@
         <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13" t="n">
         <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -955,78 +955,78 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B15" t="n">
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="K15" t="n">
         <v>0</v>
       </c>
       <c r="L15" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="B16" t="n">
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D16" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="I16" t="n">
         <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="K16" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L16" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
criando funcao para puxar as info necessarias para atualizar as informações 'por municipio' da planilha apresentação
</commit_message>
<xml_diff>
--- a/Prestador/neomater/resultado/relatorio_neomater_APENAS_VALORES.xlsx
+++ b/Prestador/neomater/resultado/relatorio_neomater_APENAS_VALORES.xlsx
@@ -423,22 +423,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E1" t="n">
         <v>0</v>
       </c>
       <c r="F1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G1" t="n">
         <v>0</v>
@@ -447,13 +447,13 @@
         <v>0</v>
       </c>
       <c r="I1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J1" t="n">
         <v>0</v>
       </c>
       <c r="K1" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L1" t="n">
         <v>0</v>
@@ -461,7 +461,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
@@ -476,25 +476,25 @@
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L2" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -546,7 +546,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -567,7 +567,7 @@
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" t="n">
         <v>0</v>
@@ -578,7 +578,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -613,22 +613,22 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -637,13 +637,13 @@
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L6" t="n">
         <v>0</v>
@@ -727,7 +727,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9" t="n">
         <v>0</v>
@@ -739,25 +739,25 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
         <v>0</v>
@@ -765,20 +765,20 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
+        <v>0</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
         <v>2</v>
       </c>
-      <c r="B10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" t="n">
-        <v>1</v>
-      </c>
       <c r="F10" t="n">
         <v>1</v>
       </c>
@@ -786,7 +786,7 @@
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
@@ -798,7 +798,7 @@
         <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -818,7 +818,7 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -836,7 +836,7 @@
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -879,7 +879,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B13" t="n">
         <v>0</v>
@@ -894,7 +894,7 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
@@ -955,7 +955,7 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B15" t="n">
         <v>0</v>
@@ -970,63 +970,63 @@
         <v>1</v>
       </c>
       <c r="F15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E16" t="n">
         <v>4</v>
       </c>
       <c r="F16" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J16" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K16" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="L16" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adicionando funcao de competencia e ano ao gerar os relatorios (bug do exel apresentação nao ser encontrado/preenchido)
</commit_message>
<xml_diff>
--- a/Prestador/neomater/resultado/relatorio_neomater_APENAS_VALORES.xlsx
+++ b/Prestador/neomater/resultado/relatorio_neomater_APENAS_VALORES.xlsx
@@ -423,22 +423,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E1" t="n">
         <v>0</v>
       </c>
       <c r="F1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G1" t="n">
         <v>0</v>
@@ -447,13 +447,13 @@
         <v>0</v>
       </c>
       <c r="I1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J1" t="n">
         <v>0</v>
       </c>
       <c r="K1" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="L1" t="n">
         <v>0</v>
@@ -461,7 +461,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
@@ -470,31 +470,31 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="K2" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
@@ -546,7 +546,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -567,7 +567,7 @@
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
         <v>0</v>
@@ -578,7 +578,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -613,22 +613,22 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -637,13 +637,13 @@
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
         <v>0</v>
@@ -727,7 +727,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B9" t="n">
         <v>0</v>
@@ -736,13 +736,13 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -754,18 +754,18 @@
         <v>0</v>
       </c>
       <c r="J9" t="n">
+        <v>4</v>
+      </c>
+      <c r="K9" t="n">
+        <v>2</v>
+      </c>
+      <c r="L9" t="n">
         <v>1</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B10" t="n">
         <v>0</v>
@@ -774,36 +774,36 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>3</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>5</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
         <v>2</v>
       </c>
-      <c r="F10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" t="n">
-        <v>1</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0</v>
-      </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B11" t="n">
         <v>0</v>
@@ -830,13 +830,13 @@
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -879,7 +879,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B13" t="n">
         <v>0</v>
@@ -894,7 +894,7 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
@@ -906,7 +906,7 @@
         <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K13" t="n">
         <v>0</v>
@@ -955,7 +955,7 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B15" t="n">
         <v>0</v>
@@ -964,13 +964,13 @@
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
@@ -982,51 +982,51 @@
         <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="K15" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L15" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="B16" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="I16" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="K16" t="n">
         <v>16</v>
       </c>
       <c r="L16" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
retornando apenas a competencia no arquivo do financeiro
</commit_message>
<xml_diff>
--- a/Prestador/neomater/resultado/relatorio_neomater_APENAS_VALORES.xlsx
+++ b/Prestador/neomater/resultado/relatorio_neomater_APENAS_VALORES.xlsx
@@ -461,40 +461,40 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="K2" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L2" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -727,45 +727,45 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
+        <v>3</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
         <v>4</v>
       </c>
-      <c r="B9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" t="n">
-        <v>1</v>
-      </c>
       <c r="I9" t="n">
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
         <v>2</v>
       </c>
       <c r="L9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B10" t="n">
         <v>0</v>
@@ -780,25 +780,25 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -812,28 +812,28 @@
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
         <v>0</v>
@@ -879,7 +879,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B13" t="n">
         <v>0</v>
@@ -894,7 +894,7 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
@@ -906,13 +906,13 @@
         <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K13" t="n">
         <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -955,78 +955,78 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B15" t="n">
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" t="n">
+        <v>2</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>8</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>5</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
         <v>4</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" t="n">
-        <v>5</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" t="n">
-        <v>8</v>
-      </c>
-      <c r="K15" t="n">
-        <v>5</v>
-      </c>
-      <c r="L15" t="n">
-        <v>8</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B16" t="n">
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D16" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="I16" t="n">
         <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="K16" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="L16" t="n">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
criando funcao que cria backup do arquivo que alimenta o pbi
</commit_message>
<xml_diff>
--- a/Prestador/neomater/resultado/relatorio_neomater_APENAS_VALORES.xlsx
+++ b/Prestador/neomater/resultado/relatorio_neomater_APENAS_VALORES.xlsx
@@ -461,40 +461,40 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
       </c>
       <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
         <v>1</v>
       </c>
-      <c r="D2" t="n">
+      <c r="F2" t="n">
         <v>4</v>
       </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>8</v>
-      </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L2" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -727,28 +727,28 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B9" t="n">
         <v>0</v>
       </c>
       <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
         <v>1</v>
       </c>
-      <c r="D9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
@@ -765,29 +765,29 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
         <v>9</v>
       </c>
-      <c r="B10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" t="n">
-        <v>4</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" t="n">
-        <v>1</v>
-      </c>
       <c r="I10" t="n">
         <v>0</v>
       </c>
@@ -795,36 +795,36 @@
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
+        <v>0</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
         <v>1</v>
       </c>
-      <c r="B11" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
-        <v>3</v>
-      </c>
       <c r="G11" t="n">
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
@@ -879,7 +879,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B13" t="n">
         <v>0</v>
@@ -894,7 +894,7 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
@@ -912,7 +912,7 @@
         <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -955,78 +955,78 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
+        <v>3</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>3</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
         <v>4</v>
       </c>
-      <c r="B15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" t="n">
-        <v>1</v>
-      </c>
-      <c r="D15" t="n">
-        <v>2</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" t="n">
-        <v>8</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" t="n">
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
         <v>5</v>
-      </c>
-      <c r="I15" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" t="n">
-        <v>1</v>
-      </c>
-      <c r="K15" t="n">
-        <v>0</v>
-      </c>
-      <c r="L15" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B16" t="n">
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>4</v>
+      </c>
+      <c r="F16" t="n">
         <v>12</v>
       </c>
-      <c r="E16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" t="n">
-        <v>20</v>
-      </c>
       <c r="G16" t="n">
         <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="I16" t="n">
         <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="K16" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="L16" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>